<commit_message>
se crean los casos de prueba en el documento y se agregan mas pasos en el gestor de ordenes
</commit_message>
<xml_diff>
--- a/docs/test-cases/gestorOrdenes.xlsx
+++ b/docs/test-cases/gestorOrdenes.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C4F09E-41AE-4B97-8BC6-D230F9CD5C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="GestorOrdenes" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,15 +19,172 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
+  <si>
+    <t>ID Caso</t>
+  </si>
+  <si>
+    <t>Nombre/ Descripcion</t>
+  </si>
+  <si>
+    <t>Tipo de prueba</t>
+  </si>
+  <si>
+    <t>Módulo</t>
+  </si>
+  <si>
+    <t>Precondiciones</t>
+  </si>
+  <si>
+    <t>Pasos a seguir</t>
+  </si>
+  <si>
+    <t>Datos de prueba</t>
+  </si>
+  <si>
+    <t>Resultado esperado</t>
+  </si>
+  <si>
+    <t>Resultado obtenido</t>
+  </si>
+  <si>
+    <t>Estado (OK/FALLA)</t>
+  </si>
+  <si>
+    <t>Automatizado</t>
+  </si>
+  <si>
+    <t>Observaciones</t>
+  </si>
+  <si>
+    <t>Positivo</t>
+  </si>
+  <si>
+    <t>eCenter</t>
+  </si>
+  <si>
+    <t>El usuario debe tener permisos para acceder a la vista</t>
+  </si>
+  <si>
+    <t>ID de cliente válido</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>CP_GESORD_001</t>
+  </si>
+  <si>
+    <t>ingreso a la vista Gestor de ordenes</t>
+  </si>
+  <si>
+    <t>1. Clic en módulo eCenter
+2. Scroll en el contenedor de aplicaciones
+3. Clic en "Gestor de ordenes"</t>
+  </si>
+  <si>
+    <t>El sistema debe redirigido correctamente la vistaGestor de ordenes</t>
+  </si>
+  <si>
+    <t>La vista Gestor de ordenes se cargó sin errores</t>
+  </si>
+  <si>
+    <t>CP_GESORD_002</t>
+  </si>
+  <si>
+    <t>Primer Filtro de búsqueda por ID_DEAL</t>
+  </si>
+  <si>
+    <t>El usuario debe haber accedido a la vista y dado clic en el botón filtros</t>
+  </si>
+  <si>
+    <t>1. Abrir modal de filtros
+2. Desplegar select de filtros
+3. Seleccionar "ID_DEAL"
+4.Diligenciar el campo de ID_DEAL
+5. Clic en "Aplicar filtros"</t>
+  </si>
+  <si>
+    <t>El sistema debe filtrar el por ideal y traer la informacion del cliente</t>
+  </si>
+  <si>
+    <t>se filtra el cliente por ideal y se muestra la informacion correctamente</t>
+  </si>
+  <si>
+    <t>CP_GESORD_003</t>
+  </si>
+  <si>
+    <t>RawData</t>
+  </si>
+  <si>
+    <t>El usuario debe haber accedido a la vista y dado clic la opcion RawData</t>
+  </si>
+  <si>
+    <t>El sistema debe abrir el modal RawData y mostrar la informacion correctamente</t>
+  </si>
+  <si>
+    <t>se abre el modal correctamente y se muestra la informacion</t>
+  </si>
+  <si>
+    <t>Adjuntos</t>
+  </si>
+  <si>
+    <t>eProvisionig</t>
+  </si>
+  <si>
+    <t>CP_GESORD_004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Seleccionar cliente
+2.Abrir menú de opciones
+3.Seleccionar opción "Adjuntos"
+4.Clic en el botón "Refrescar" dentro del modal Adjuntos
+5.Clic en el botón "Cerrar" dentro del modal Adjuntos
+</t>
+  </si>
+  <si>
+    <t>1.Seleccionar cliente
+2.Abrir menú de opciones
+3.Seleccionar opción "RawData"
+4.Hacer scroll hacia abajo dentro del contenedor RawData
+5.Clic en el botón "Copiar"
+6.Clic en el botón "Cerrar"</t>
+  </si>
+  <si>
+    <t>El sistema debe abrir el modal Adjuntos y mostrar la informacion correctamente</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +195,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -45,12 +203,113 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +589,220 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25" customWidth="1"/>
+    <col min="8" max="8" width="27.5703125" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" customWidth="1"/>
+    <col min="10" max="10" width="28" customWidth="1"/>
+    <col min="11" max="11" width="27.85546875" customWidth="1"/>
+    <col min="12" max="12" width="35.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>